<commit_message>
Task 3 - Removed More Duplicates & Fixed Names
</commit_message>
<xml_diff>
--- a/data-cleaning-excel-tutorial - Cleaned.xlsx
+++ b/data-cleaning-excel-tutorial - Cleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\DATA SCIENCE\EXCEL Data Cleaning\Excel-Data-Cleaning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBCA2E4-038D-425B-A4E8-86CD7A956F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3309B9C7-30D4-4F27-9BC9-A98E2AD0C76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="138">
   <si>
     <t>S.No.</t>
   </si>
@@ -446,6 +446,9 @@
   </si>
   <si>
     <t>date updated</t>
+  </si>
+  <si>
+    <t>president-fixed</t>
   </si>
 </sst>
 </file>
@@ -1300,18 +1303,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:XFD46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="23.5546875" style="3"/>
+    <col min="8" max="8" width="23.5546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1319,25 +1322,28 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>136</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1347,26 +1353,30 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="str">
+        <f>PROPER(C2)</f>
+        <v>George Washington</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>131</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2" s="4">
         <v>5000</v>
       </c>
-      <c r="H2" s="1">
-        <v>44391</v>
-      </c>
       <c r="I2" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J2" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1376,26 +1386,30 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D47" si="0">PROPER(C3)</f>
+        <v>John Adams</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>10000</v>
       </c>
-      <c r="H3" s="1">
-        <v>44391</v>
-      </c>
       <c r="I3" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J3" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1405,26 +1419,30 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>Thomas Jefferson</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>15000</v>
       </c>
-      <c r="H4" s="1">
-        <v>44391</v>
-      </c>
       <c r="I4" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J4" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1434,26 +1452,30 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>James Madison</v>
+      </c>
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="4">
+      <c r="H5" s="4">
         <v>20000</v>
       </c>
-      <c r="H5" s="1">
-        <v>44391</v>
-      </c>
       <c r="I5" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J5" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1463,26 +1485,30 @@
       <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>James Monroe</v>
+      </c>
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="4">
         <v>25000</v>
       </c>
-      <c r="H6" s="1">
-        <v>44391</v>
-      </c>
       <c r="I6" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J6" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1492,26 +1518,30 @@
       <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>John Quincy Adams</v>
+      </c>
+      <c r="E7" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="4">
+      <c r="H7" s="4">
         <v>30000</v>
       </c>
-      <c r="H7" s="1">
-        <v>44391</v>
-      </c>
       <c r="I7" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J7" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1521,26 +1551,30 @@
       <c r="C8" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>Andrew Jackson</v>
+      </c>
+      <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>26</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="4">
+      <c r="H8" s="4">
         <v>35000</v>
       </c>
-      <c r="H8" s="1">
-        <v>44391</v>
-      </c>
       <c r="I8" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J8" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1550,26 +1584,30 @@
       <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>Martin Van Buren</v>
+      </c>
+      <c r="E9" t="s">
         <v>29</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>26</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="4">
+      <c r="H9" s="4">
         <v>40000</v>
       </c>
-      <c r="H9" s="1">
-        <v>44391</v>
-      </c>
       <c r="I9" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J9" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1579,26 +1617,30 @@
       <c r="C10" t="s">
         <v>31</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>William Henry Harrison</v>
+      </c>
+      <c r="E10" t="s">
         <v>32</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>33</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="4">
+      <c r="H10" s="4">
         <v>45000</v>
       </c>
-      <c r="H10" s="1">
-        <v>44391</v>
-      </c>
       <c r="I10" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J10" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1608,26 +1650,30 @@
       <c r="C11" t="s">
         <v>35</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>John Tyler</v>
+      </c>
+      <c r="E11" t="s">
         <v>36</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>37</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="4">
+      <c r="H11" s="4">
         <v>50000</v>
       </c>
-      <c r="H11" s="1">
-        <v>44391</v>
-      </c>
       <c r="I11" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J11" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1637,26 +1683,30 @@
       <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>James K. Polk</v>
+      </c>
+      <c r="E12" t="s">
         <v>40</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>26</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="4">
+      <c r="H12" s="4">
         <v>55000</v>
       </c>
-      <c r="H12" s="1">
-        <v>44391</v>
-      </c>
       <c r="I12" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J12" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1666,26 +1716,30 @@
       <c r="C13" t="s">
         <v>42</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>Zachary Taylor</v>
+      </c>
+      <c r="E13" t="s">
         <v>43</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>33</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="4">
+      <c r="H13" s="4">
         <v>60000</v>
       </c>
-      <c r="H13" s="1">
-        <v>44391</v>
-      </c>
       <c r="I13" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J13" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1695,26 +1749,30 @@
       <c r="C14" t="s">
         <v>45</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>Millard Fillmore</v>
+      </c>
+      <c r="E14" t="s">
         <v>46</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>33</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="4">
+      <c r="H14" s="4">
         <v>65000</v>
       </c>
-      <c r="H14" s="1">
-        <v>44391</v>
-      </c>
       <c r="I14" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J14" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1724,26 +1782,30 @@
       <c r="C15" t="s">
         <v>47</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>Franklin Pierce</v>
+      </c>
+      <c r="E15" t="s">
         <v>48</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>26</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="4">
+      <c r="H15" s="4">
         <v>75000</v>
       </c>
-      <c r="H15" s="1">
-        <v>44391</v>
-      </c>
       <c r="I15" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J15" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1753,26 +1815,30 @@
       <c r="C16" t="s">
         <v>50</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>James Buchanan</v>
+      </c>
+      <c r="E16" t="s">
         <v>51</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>26</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>52</v>
       </c>
-      <c r="G16" s="4">
+      <c r="H16" s="4">
         <v>85000</v>
       </c>
-      <c r="H16" s="1">
-        <v>44391</v>
-      </c>
       <c r="I16" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J16" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1782,26 +1848,30 @@
       <c r="C17" t="s">
         <v>53</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>Abraham Lincoln</v>
+      </c>
+      <c r="E17" t="s">
         <v>54</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>60</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>55</v>
       </c>
-      <c r="G17" s="4">
+      <c r="H17" s="4">
         <v>95000</v>
       </c>
-      <c r="H17" s="1">
-        <v>44391</v>
-      </c>
       <c r="I17" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J17" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1811,26 +1881,30 @@
       <c r="C18" t="s">
         <v>56</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>Andrew Johnson</v>
+      </c>
+      <c r="E18" t="s">
         <v>57</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>26</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="4">
+      <c r="H18" s="4">
         <v>105000</v>
       </c>
-      <c r="H18" s="1">
-        <v>44391</v>
-      </c>
       <c r="I18" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J18" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1840,26 +1914,30 @@
       <c r="C19" t="s">
         <v>58</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>Ulysses S. Grant</v>
+      </c>
+      <c r="E19" t="s">
         <v>59</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>60</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>61</v>
       </c>
-      <c r="G19" s="4">
+      <c r="H19" s="4">
         <v>115000</v>
       </c>
-      <c r="H19" s="1">
-        <v>44391</v>
-      </c>
       <c r="I19" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J19" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1869,26 +1947,30 @@
       <c r="C20" t="s">
         <v>62</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>Rutherford B. Hayes</v>
+      </c>
+      <c r="E20" t="s">
         <v>63</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>60</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>64</v>
       </c>
-      <c r="G20" s="4">
+      <c r="H20" s="4">
         <v>125000</v>
       </c>
-      <c r="H20" s="1">
-        <v>44391</v>
-      </c>
       <c r="I20" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J20" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1898,26 +1980,30 @@
       <c r="C21" t="s">
         <v>65</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>James A. Garfield</v>
+      </c>
+      <c r="E21" t="s">
         <v>66</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>60</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>67</v>
       </c>
-      <c r="G21" s="4">
+      <c r="H21" s="4">
         <v>135000</v>
       </c>
-      <c r="H21" s="1">
-        <v>44391</v>
-      </c>
       <c r="I21" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J21" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1927,26 +2013,30 @@
       <c r="C22" t="s">
         <v>67</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>Chester A. Arthur</v>
+      </c>
+      <c r="E22" t="s">
         <v>68</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>60</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="4">
+      <c r="H22" s="4">
         <v>145000</v>
       </c>
-      <c r="H22" s="1">
-        <v>44391</v>
-      </c>
       <c r="I22" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J22" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1956,26 +2046,30 @@
       <c r="C23" t="s">
         <v>69</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>Grover Cleveland</v>
+      </c>
+      <c r="E23" t="s">
         <v>70</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>26</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>71</v>
       </c>
-      <c r="G23" s="4">
+      <c r="H23" s="4">
         <v>155000</v>
       </c>
-      <c r="H23" s="1">
-        <v>44391</v>
-      </c>
       <c r="I23" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J23" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1985,26 +2079,30 @@
       <c r="C24" t="s">
         <v>72</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>Benjamin Harrison</v>
+      </c>
+      <c r="E24" t="s">
         <v>73</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>60</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>74</v>
       </c>
-      <c r="G24" s="4">
+      <c r="H24" s="4">
         <v>165000</v>
       </c>
-      <c r="H24" s="1">
-        <v>44391</v>
-      </c>
       <c r="I24" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J24" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2014,26 +2112,30 @@
       <c r="C25" t="s">
         <v>69</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>Grover Cleveland</v>
+      </c>
+      <c r="E25" t="s">
         <v>75</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>26</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>76</v>
       </c>
-      <c r="G25" s="4">
+      <c r="H25" s="4">
         <v>175000</v>
       </c>
-      <c r="H25" s="1">
-        <v>44391</v>
-      </c>
       <c r="I25" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J25" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2043,26 +2145,30 @@
       <c r="C26" t="s">
         <v>77</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>William Mckinley</v>
+      </c>
+      <c r="E26" t="s">
         <v>78</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>60</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>79</v>
       </c>
-      <c r="G26" s="4">
+      <c r="H26" s="4">
         <v>185000</v>
       </c>
-      <c r="H26" s="1">
-        <v>44391</v>
-      </c>
       <c r="I26" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J26" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2072,26 +2178,30 @@
       <c r="C27" t="s">
         <v>80</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>Theodore Roosevelt</v>
+      </c>
+      <c r="E27" t="s">
         <v>81</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>60</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>38</v>
       </c>
-      <c r="G27" s="4">
+      <c r="H27" s="4">
         <v>195000</v>
       </c>
-      <c r="H27" s="1">
-        <v>44391</v>
-      </c>
       <c r="I27" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J27" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2101,26 +2211,30 @@
       <c r="C28" t="s">
         <v>82</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>William Howard Taft</v>
+      </c>
+      <c r="E28" t="s">
         <v>83</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>60</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>84</v>
       </c>
-      <c r="G28" s="4">
+      <c r="H28" s="4">
         <v>205000</v>
       </c>
-      <c r="H28" s="1">
-        <v>44391</v>
-      </c>
       <c r="I28" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J28" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2130,26 +2244,30 @@
       <c r="C29" t="s">
         <v>85</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>Woodrow Wilson</v>
+      </c>
+      <c r="E29" t="s">
         <v>86</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>26</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>87</v>
       </c>
-      <c r="G29" s="4">
+      <c r="H29" s="4">
         <v>225000</v>
       </c>
-      <c r="H29" s="1">
-        <v>44391</v>
-      </c>
       <c r="I29" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J29" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2159,26 +2277,30 @@
       <c r="C30" t="s">
         <v>85</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>Woodrow Wilson</v>
+      </c>
+      <c r="E30" t="s">
         <v>86</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>133</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>87</v>
       </c>
-      <c r="G30" s="4">
+      <c r="H30" s="4">
         <v>225000</v>
       </c>
-      <c r="H30" s="1">
-        <v>44391</v>
-      </c>
       <c r="I30" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J30" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>28</v>
       </c>
@@ -2188,26 +2310,30 @@
       <c r="C31" t="s">
         <v>88</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>Warren G. Harding</v>
+      </c>
+      <c r="E31" t="s">
         <v>89</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>60</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>90</v>
       </c>
-      <c r="G31" s="4">
+      <c r="H31" s="4">
         <v>235000</v>
       </c>
-      <c r="H31" s="1">
-        <v>44391</v>
-      </c>
       <c r="I31" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J31" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2217,26 +2343,30 @@
       <c r="C32" t="s">
         <v>90</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>Calvin Coolidge</v>
+      </c>
+      <c r="E32" t="s">
         <v>91</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>60</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>38</v>
       </c>
-      <c r="G32" s="4">
+      <c r="H32" s="4">
         <v>245000</v>
       </c>
-      <c r="H32" s="1">
-        <v>44391</v>
-      </c>
       <c r="I32" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J32" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2246,26 +2376,30 @@
       <c r="C33" t="s">
         <v>92</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>Herbert Hoover</v>
+      </c>
+      <c r="E33" t="s">
         <v>93</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>60</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>94</v>
       </c>
-      <c r="G33" s="4">
+      <c r="H33" s="4">
         <v>255000</v>
       </c>
-      <c r="H33" s="1">
-        <v>44391</v>
-      </c>
       <c r="I33" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J33" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>31</v>
       </c>
@@ -2275,26 +2409,30 @@
       <c r="C34" t="s">
         <v>95</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>Franklin D. Roosevelt</v>
+      </c>
+      <c r="E34" t="s">
         <v>96</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>26</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>97</v>
       </c>
-      <c r="G34" s="4">
+      <c r="H34" s="4">
         <v>265000</v>
       </c>
-      <c r="H34" s="1">
-        <v>44391</v>
-      </c>
       <c r="I34" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J34" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>32</v>
       </c>
@@ -2304,26 +2442,30 @@
       <c r="C35" t="s">
         <v>98</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>Harry S. Truman</v>
+      </c>
+      <c r="E35" t="s">
         <v>99</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>26</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>38</v>
       </c>
-      <c r="G35" s="4">
+      <c r="H35" s="4">
         <v>275000</v>
       </c>
-      <c r="H35" s="1">
-        <v>44391</v>
-      </c>
       <c r="I35" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J35" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>33</v>
       </c>
@@ -2333,26 +2475,30 @@
       <c r="C36" t="s">
         <v>100</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>Dwight D. Eisenhower</v>
+      </c>
+      <c r="E36" t="s">
         <v>101</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>60</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>102</v>
       </c>
-      <c r="G36" s="4">
+      <c r="H36" s="4">
         <v>285000</v>
       </c>
-      <c r="H36" s="1">
-        <v>44391</v>
-      </c>
       <c r="I36" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J36" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>34</v>
       </c>
@@ -2362,26 +2508,30 @@
       <c r="C37" t="s">
         <v>103</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>John F. Kennedy</v>
+      </c>
+      <c r="E37" t="s">
         <v>104</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>26</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>105</v>
       </c>
-      <c r="G37" s="4">
+      <c r="H37" s="4">
         <v>295000</v>
       </c>
-      <c r="H37" s="1">
-        <v>44391</v>
-      </c>
       <c r="I37" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J37" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>35</v>
       </c>
@@ -2391,26 +2541,30 @@
       <c r="C38" t="s">
         <v>105</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>Lyndon B. Johnson</v>
+      </c>
+      <c r="E38" t="s">
         <v>106</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>26</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>38</v>
       </c>
-      <c r="G38" s="4">
+      <c r="H38" s="4">
         <v>305000</v>
       </c>
-      <c r="H38" s="1">
-        <v>44391</v>
-      </c>
       <c r="I38" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J38" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>36</v>
       </c>
@@ -2420,26 +2574,30 @@
       <c r="C39" t="s">
         <v>102</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>Richard Nixon</v>
+      </c>
+      <c r="E39" t="s">
         <v>107</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>60</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>108</v>
       </c>
-      <c r="G39" s="4">
+      <c r="H39" s="4">
         <v>315000</v>
       </c>
-      <c r="H39" s="1">
-        <v>44391</v>
-      </c>
       <c r="I39" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J39" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>37</v>
       </c>
@@ -2449,26 +2607,30 @@
       <c r="C40" t="s">
         <v>109</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>Gerald Ford</v>
+      </c>
+      <c r="E40" t="s">
         <v>110</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>60</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>38</v>
       </c>
-      <c r="G40" s="4">
+      <c r="H40" s="4">
         <v>325000</v>
       </c>
-      <c r="H40" s="1">
-        <v>44391</v>
-      </c>
       <c r="I40" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J40" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>38</v>
       </c>
@@ -2478,26 +2640,30 @@
       <c r="C41" t="s">
         <v>111</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>Jimmy Carter</v>
+      </c>
+      <c r="E41" t="s">
         <v>112</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>26</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>113</v>
       </c>
-      <c r="G41" s="4">
+      <c r="H41" s="4">
         <v>335000</v>
       </c>
-      <c r="H41" s="1">
-        <v>44391</v>
-      </c>
       <c r="I41" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J41" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>39</v>
       </c>
@@ -2507,26 +2673,30 @@
       <c r="C42" t="s">
         <v>114</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>Ronald Reagan</v>
+      </c>
+      <c r="E42" t="s">
         <v>115</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>60</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>116</v>
       </c>
-      <c r="G42" s="4">
+      <c r="H42" s="4">
         <v>345000</v>
       </c>
-      <c r="H42" s="1">
-        <v>44391</v>
-      </c>
       <c r="I42" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J42" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>40</v>
       </c>
@@ -2536,26 +2706,30 @@
       <c r="C43" t="s">
         <v>116</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>George H. W. Bush</v>
+      </c>
+      <c r="E43" t="s">
         <v>117</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>60</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>118</v>
       </c>
-      <c r="G43" s="4">
+      <c r="H43" s="4">
         <v>355000</v>
       </c>
-      <c r="H43" s="1">
-        <v>44391</v>
-      </c>
       <c r="I43" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J43" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>41</v>
       </c>
@@ -2565,26 +2739,30 @@
       <c r="C44" t="s">
         <v>119</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>Bill Clinton</v>
+      </c>
+      <c r="E44" t="s">
         <v>120</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>26</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>121</v>
       </c>
-      <c r="G44" s="4">
+      <c r="H44" s="4">
         <v>365000</v>
       </c>
-      <c r="H44" s="1">
-        <v>44391</v>
-      </c>
       <c r="I44" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J44" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>42</v>
       </c>
@@ -2594,26 +2772,30 @@
       <c r="C45" t="s">
         <v>122</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>George W. Bush</v>
+      </c>
+      <c r="E45" t="s">
         <v>123</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>60</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>124</v>
       </c>
-      <c r="G45" s="4">
+      <c r="H45" s="4">
         <v>375000</v>
       </c>
-      <c r="H45" s="1">
-        <v>44391</v>
-      </c>
       <c r="I45" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44391</v>
+      </c>
+      <c r="J45" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>43</v>
       </c>
@@ -2623,85 +2805,67 @@
       <c r="C46" t="s">
         <v>125</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>Barack Obama</v>
+      </c>
+      <c r="E46" t="s">
         <v>126</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>26</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>127</v>
       </c>
-      <c r="G46" s="4">
+      <c r="H46" s="4">
         <v>395000</v>
       </c>
-      <c r="H46" s="2">
-        <v>44391</v>
-      </c>
       <c r="I46" s="2">
+        <v>44391</v>
+      </c>
+      <c r="J46" s="2">
         <v>43862</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B47">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>125</v>
-      </c>
-      <c r="D47" t="s">
-        <v>126</v>
+        <v>128</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>Donald Trump</v>
       </c>
       <c r="E47" t="s">
-        <v>26</v>
+        <v>129</v>
       </c>
       <c r="F47" t="s">
-        <v>127</v>
-      </c>
-      <c r="G47" s="4">
-        <v>395000</v>
-      </c>
-      <c r="H47" s="2">
-        <v>44391</v>
+        <v>132</v>
+      </c>
+      <c r="G47" t="s">
+        <v>130</v>
+      </c>
+      <c r="H47" s="4">
+        <v>405000</v>
       </c>
       <c r="I47" s="2">
+        <v>44391</v>
+      </c>
+      <c r="J47" s="2">
         <v>43862</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>44</v>
-      </c>
-      <c r="B48">
-        <v>45</v>
-      </c>
-      <c r="C48" t="s">
-        <v>128</v>
-      </c>
-      <c r="D48" t="s">
-        <v>129</v>
-      </c>
-      <c r="E48" t="s">
-        <v>132</v>
-      </c>
-      <c r="F48" t="s">
-        <v>130</v>
-      </c>
-      <c r="G48" s="4">
-        <v>405000</v>
-      </c>
-      <c r="H48" s="2">
-        <v>44391</v>
-      </c>
-      <c r="I48" s="2">
-        <v>43862</v>
-      </c>
-    </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G49"/>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H48"/>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H49"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>